<commit_message>
[FieldGroup] FieldGroup Upgrade UI 레벨업 효과 적용
</commit_message>
<xml_diff>
--- a/DataTable/FieldGroupLevelTable.xlsx
+++ b/DataTable/FieldGroupLevelTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{45027730-0F5F-0944-929A-B87447952547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{585C88E7-8AB8-D741-B8B3-D9D4E0CC1FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="1040" windowWidth="16880" windowHeight="9700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7480" yWindow="-15980" windowWidth="18960" windowHeight="11420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FieldGroupLevelTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="8" uniqueCount="5">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="16" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -53,6 +53,26 @@
   </si>
   <si>
     <t>gem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>noneGradeRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bronzeGradeRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>silverGradeRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldGradeRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1035,107 +1055,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D17"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5703125" style="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="G4" s="3">
         <v>5000</v>
       </c>
-      <c r="D4" s="3">
+      <c r="H4" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <f>A4+1</f>
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
         <v>5000</v>
       </c>
-      <c r="D5" s="3">
+      <c r="H5" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
         <f t="shared" ref="A6:A17" si="0">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3">
         <v>5000</v>
       </c>
-      <c r="D6" s="3">
+      <c r="H6" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
         <v>5000</v>
       </c>
-      <c r="D7" s="3">
+      <c r="H7" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:8">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1144,144 +1240,264 @@
         <v>4</v>
       </c>
       <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
         <v>5000</v>
       </c>
-      <c r="D8" s="3">
+      <c r="H8" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:8">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="G9" s="3">
         <v>5000</v>
       </c>
-      <c r="D9" s="3">
+      <c r="H9" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:8">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B10" s="3">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="3">
+      <c r="G10" s="3">
         <v>5000</v>
       </c>
-      <c r="D10" s="3">
+      <c r="H10" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:8">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="3">
+      <c r="G11" s="3">
         <v>5000</v>
       </c>
-      <c r="D11" s="3">
+      <c r="H11" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:8">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="3">
+      <c r="G12" s="3">
         <v>5000</v>
       </c>
-      <c r="D12" s="3">
+      <c r="H12" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:8">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="3">
+      <c r="G13" s="3">
         <v>5000</v>
       </c>
-      <c r="D13" s="3">
+      <c r="H13" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:8">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="3">
+      <c r="G14" s="3">
         <v>5000</v>
       </c>
-      <c r="D14" s="3">
+      <c r="H14" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:8">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B15" s="3">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
         <v>11</v>
       </c>
-      <c r="C15" s="3">
+      <c r="G15" s="3">
         <v>5000</v>
       </c>
-      <c r="D15" s="3">
+      <c r="H15" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:8">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B16" s="3">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="3">
+      <c r="G16" s="3">
         <v>5000</v>
       </c>
-      <c r="D16" s="3">
+      <c r="H16" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:8">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B17" s="3">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="3">
+      <c r="G17" s="3">
         <v>5000</v>
       </c>
-      <c r="D17" s="3">
+      <c r="H17" s="3">
         <v>100</v>
       </c>
     </row>

</xml_diff>